<commit_message>
Corrected the 20% weight difference to percent error equation
</commit_message>
<xml_diff>
--- a/Summary CATE Metrics_05.08.2023.xlsx
+++ b/Summary CATE Metrics_05.08.2023.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shelbygolden/Desktop/Life/Personal/College/Masters/Johns Hopkins/Statistical Theory II/Stat Theory II_Spring 2023/Semester Project/Project GitHub Repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630CD07-1A91-154F-8B79-D823FDFD43C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E9B15E-F73D-8643-8113-92298F149447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{60BB6ECC-ECB2-534B-AD4D-AA5F7D624C1A}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{60BB6ECC-ECB2-534B-AD4D-AA5F7D624C1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -151,7 +151,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -218,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -251,7 +251,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -571,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E079E24D-2813-5649-8A03-9BB3068BA1C6}">
-  <dimension ref="B2:K29"/>
+  <dimension ref="B2:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,26 +1014,44 @@
         <v>28</v>
       </c>
     </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F26" s="18"/>
+    </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="11"/>
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="11"/>
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="11"/>
       <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F30" s="18"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B26:J27">

</xml_diff>